<commit_message>
Finished decision tree and neural network
</commit_message>
<xml_diff>
--- a/results/decisiontree.xlsx
+++ b/results/decisiontree.xlsx
@@ -529,52 +529,52 @@
         <v>0.5671641791044776</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4328358208955224</v>
+        <v>0.5671641791044776</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6567164179104478</v>
+        <v>0.5671641791044776</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6417910447761194</v>
+        <v>0.5671641791044776</v>
       </c>
       <c r="I2" t="n">
-        <v>0.6567164179104478</v>
+        <v>0.5671641791044776</v>
       </c>
       <c r="J2" t="n">
+        <v>0.7313432835820896</v>
+      </c>
+      <c r="K2" t="n">
         <v>0.835820895522388</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.746268656716418</v>
       </c>
       <c r="L2" t="n">
         <v>0.835820895522388</v>
       </c>
       <c r="M2" t="n">
-        <v>0.835820895522388</v>
+        <v>0.7313432835820896</v>
       </c>
       <c r="N2" t="n">
         <v>0.835820895522388</v>
       </c>
       <c r="O2" t="n">
-        <v>0.7611940298507462</v>
+        <v>0.835820895522388</v>
       </c>
       <c r="P2" t="n">
-        <v>0.7910447761194029</v>
+        <v>0.835820895522388</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.7164179104477612</v>
+        <v>0.835820895522388</v>
       </c>
       <c r="R2" t="n">
-        <v>0.7164179104477612</v>
+        <v>0.835820895522388</v>
       </c>
       <c r="S2" t="n">
-        <v>0.7910447761194029</v>
+        <v>0.835820895522388</v>
       </c>
       <c r="T2" t="n">
-        <v>0.8507462686567164</v>
+        <v>0.7313432835820896</v>
       </c>
       <c r="U2" t="n">
-        <v>0.8507462686567164</v>
+        <v>0.7761194029850746</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -586,58 +586,58 @@
         <v>0.5671641791044776</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5671641791044776</v>
+        <v>0.7611940298507462</v>
       </c>
       <c r="E3" t="n">
         <v>0.5671641791044776</v>
       </c>
       <c r="F3" t="n">
+        <v>0.5522388059701493</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.5074626865671642</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.835820895522388</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.6716417910447762</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.5373134328358209</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.5373134328358209</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.5373134328358209</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.5373134328358209</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.8208955223880597</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.835820895522388</v>
+      </c>
+      <c r="P3" t="n">
         <v>0.5671641791044776</v>
       </c>
-      <c r="G3" t="n">
-        <v>0.6417910447761194</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.7611940298507462</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.6567164179104478</v>
-      </c>
-      <c r="J3" t="n">
+      <c r="Q3" t="n">
         <v>0.835820895522388</v>
       </c>
-      <c r="K3" t="n">
+      <c r="R3" t="n">
         <v>0.8059701492537313</v>
       </c>
-      <c r="L3" t="n">
-        <v>0.7014925373134329</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.8059701492537313</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.8507462686567164</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0.8507462686567164</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0.8507462686567164</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0.8059701492537313</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0.8507462686567164</v>
-      </c>
       <c r="S3" t="n">
-        <v>0.8507462686567164</v>
+        <v>0.835820895522388</v>
       </c>
       <c r="T3" t="n">
-        <v>0.8656716417910447</v>
+        <v>0.7761194029850746</v>
       </c>
       <c r="U3" t="n">
-        <v>0.8507462686567164</v>
+        <v>0.8208955223880597</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -649,37 +649,37 @@
         <v>0.4328358208955224</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5223880597014925</v>
+        <v>0.7313432835820896</v>
       </c>
       <c r="E4" t="n">
+        <v>0.6567164179104478</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.7014925373134329</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.7014925373134329</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.746268656716418</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.8208955223880597</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.8208955223880597</v>
+      </c>
+      <c r="K4" t="n">
         <v>0.7611940298507462</v>
       </c>
-      <c r="F4" t="n">
-        <v>0.5671641791044776</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.5970149253731343</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.7611940298507462</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.7611940298507462</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.6716417910447762</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.6716417910447762</v>
-      </c>
       <c r="L4" t="n">
-        <v>0.6716417910447762</v>
+        <v>0.8208955223880597</v>
       </c>
       <c r="M4" t="n">
-        <v>0.746268656716418</v>
+        <v>0.835820895522388</v>
       </c>
       <c r="N4" t="n">
-        <v>0.6716417910447762</v>
+        <v>0.835820895522388</v>
       </c>
       <c r="O4" t="n">
         <v>0.835820895522388</v>
@@ -709,55 +709,55 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4328358208955224</v>
+        <v>0.5671641791044776</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4328358208955224</v>
+        <v>0.5671641791044776</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8208955223880597</v>
+        <v>0.5671641791044776</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4626865671641791</v>
+        <v>0.5671641791044776</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5970149253731343</v>
+        <v>0.5671641791044776</v>
       </c>
       <c r="H5" t="n">
         <v>0.5671641791044776</v>
       </c>
       <c r="I5" t="n">
-        <v>0.5671641791044776</v>
+        <v>0.835820895522388</v>
       </c>
       <c r="J5" t="n">
-        <v>0.6567164179104478</v>
+        <v>0.7761194029850746</v>
       </c>
       <c r="K5" t="n">
-        <v>0.5373134328358209</v>
+        <v>0.7761194029850746</v>
       </c>
       <c r="L5" t="n">
-        <v>0.7164179104477612</v>
+        <v>0.7014925373134329</v>
       </c>
       <c r="M5" t="n">
-        <v>0.6417910447761194</v>
+        <v>0.835820895522388</v>
       </c>
       <c r="N5" t="n">
-        <v>0.746268656716418</v>
+        <v>0.835820895522388</v>
       </c>
       <c r="O5" t="n">
+        <v>0.7910447761194029</v>
+      </c>
+      <c r="P5" t="n">
         <v>0.7611940298507462</v>
       </c>
-      <c r="P5" t="n">
-        <v>0.7761194029850746</v>
-      </c>
       <c r="Q5" t="n">
-        <v>0.746268656716418</v>
+        <v>0.7910447761194029</v>
       </c>
       <c r="R5" t="n">
-        <v>0.6716417910447762</v>
+        <v>0.7910447761194029</v>
       </c>
       <c r="S5" t="n">
-        <v>0.8507462686567164</v>
+        <v>0.7611940298507462</v>
       </c>
       <c r="T5" t="n">
         <v>0.7910447761194029</v>
@@ -772,61 +772,61 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
+        <v>0.4328358208955224</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.4328358208955224</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.582089552238806</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.6716417910447762</v>
+      </c>
+      <c r="G6" t="n">
         <v>0.5671641791044776</v>
       </c>
-      <c r="D6" t="n">
-        <v>0.5671641791044776</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.5671641791044776</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.5671641791044776</v>
-      </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>0.7014925373134329</v>
       </c>
-      <c r="H6" t="n">
-        <v>0.7164179104477612</v>
-      </c>
       <c r="I6" t="n">
-        <v>0.8059701492537313</v>
+        <v>0.7611940298507462</v>
       </c>
       <c r="J6" t="n">
         <v>0.7164179104477612</v>
       </c>
       <c r="K6" t="n">
-        <v>0.7164179104477612</v>
+        <v>0.582089552238806</v>
       </c>
       <c r="L6" t="n">
+        <v>0.8059701492537313</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.8059701492537313</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.6865671641791045</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.7611940298507462</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.8059701492537313</v>
+      </c>
+      <c r="Q6" t="n">
         <v>0.7761194029850746</v>
       </c>
-      <c r="M6" t="n">
+      <c r="R6" t="n">
+        <v>0.6716417910447762</v>
+      </c>
+      <c r="S6" t="n">
         <v>0.7014925373134329</v>
       </c>
-      <c r="N6" t="n">
-        <v>0.7014925373134329</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0.7014925373134329</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0.7164179104477612</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0.7014925373134329</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0.7761194029850746</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0.7910447761194029</v>
-      </c>
       <c r="T6" t="n">
-        <v>0.7761194029850746</v>
+        <v>0.6865671641791045</v>
       </c>
       <c r="U6" t="n">
-        <v>0.7761194029850746</v>
+        <v>0.6865671641791045</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -838,58 +838,58 @@
         <v>0.5134328358208955</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5313432835820895</v>
+        <v>0.6119402985074627</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6567164179104477</v>
+        <v>0.5880597014925373</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5194029850746268</v>
+        <v>0.6119402985074627</v>
       </c>
       <c r="G7" t="n">
-        <v>0.6388059701492537</v>
+        <v>0.5820895522388059</v>
       </c>
       <c r="H7" t="n">
-        <v>0.6895522388059702</v>
+        <v>0.6835820895522388</v>
       </c>
       <c r="I7" t="n">
-        <v>0.6895522388059702</v>
+        <v>0.7313432835820896</v>
       </c>
       <c r="J7" t="n">
-        <v>0.7432835820895523</v>
+        <v>0.7164179104477612</v>
       </c>
       <c r="K7" t="n">
-        <v>0.6955223880597015</v>
+        <v>0.6985074626865672</v>
       </c>
       <c r="L7" t="n">
         <v>0.7402985074626866</v>
       </c>
       <c r="M7" t="n">
-        <v>0.7462686567164178</v>
+        <v>0.7492537313432835</v>
       </c>
       <c r="N7" t="n">
-        <v>0.7611940298507462</v>
+        <v>0.8029850746268655</v>
       </c>
       <c r="O7" t="n">
-        <v>0.7820895522388061</v>
+        <v>0.8119402985074627</v>
       </c>
       <c r="P7" t="n">
+        <v>0.7432835820895523</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.7999999999999999</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.7880597014925372</v>
+      </c>
+      <c r="S7" t="n">
         <v>0.7761194029850745</v>
       </c>
-      <c r="Q7" t="n">
-        <v>0.7462686567164178</v>
-      </c>
-      <c r="R7" t="n">
-        <v>0.7701492537313432</v>
-      </c>
-      <c r="S7" t="n">
-        <v>0.8059701492537312</v>
-      </c>
       <c r="T7" t="n">
-        <v>0.8089552238805968</v>
+        <v>0.7492537313432835</v>
       </c>
       <c r="U7" t="n">
-        <v>0.8029850746268657</v>
+        <v>0.7641791044776118</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -901,58 +901,58 @@
         <v>0.06580718711954807</v>
       </c>
       <c r="D8" t="n">
-        <v>0.05221747965533105</v>
+        <v>0.1205171894817096</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1112916530287</v>
+        <v>0.03481165310355405</v>
       </c>
       <c r="F8" t="n">
-        <v>0.05925203952620658</v>
+        <v>0.06189982493530665</v>
       </c>
       <c r="G8" t="n">
-        <v>0.03937583868141173</v>
+        <v>0.0640227181776932</v>
       </c>
       <c r="H8" t="n">
-        <v>0.07516225857918908</v>
+        <v>0.1044349593106621</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0846414739030318</v>
+        <v>0.1003446944117708</v>
       </c>
       <c r="J8" t="n">
-        <v>0.07806983182460905</v>
+        <v>0.09672747311056509</v>
       </c>
       <c r="K8" t="n">
-        <v>0.09034475194281526</v>
+        <v>0.1169143643436784</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0586474110578761</v>
+        <v>0.1119303478164339</v>
       </c>
       <c r="M8" t="n">
-        <v>0.07000620537049894</v>
+        <v>0.1126445508305266</v>
       </c>
       <c r="N8" t="n">
-        <v>0.07126767991828847</v>
+        <v>0.05849527743959829</v>
       </c>
       <c r="O8" t="n">
-        <v>0.05471732173081599</v>
+        <v>0.03073322430145373</v>
       </c>
       <c r="P8" t="n">
-        <v>0.0452708981734421</v>
+        <v>0.09363813218721267</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.03655954839974893</v>
+        <v>0.03073322430145373</v>
       </c>
       <c r="R8" t="n">
-        <v>0.06846176084286396</v>
+        <v>0.06073728343097252</v>
       </c>
       <c r="S8" t="n">
-        <v>0.04004897870148877</v>
+        <v>0.05255766227360896</v>
       </c>
       <c r="T8" t="n">
-        <v>0.04157727843935557</v>
+        <v>0.03704380192833091</v>
       </c>
       <c r="U8" t="n">
-        <v>0.04157727843935557</v>
+        <v>0.04566286131575629</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -966,58 +966,58 @@
         <v>0.5555555555555556</v>
       </c>
       <c r="D9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.7638888888888888</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.7638888888888888</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.8055555555555556</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.6111111111111112</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.7638888888888888</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.6527777777777778</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.7916666666666666</v>
+      </c>
+      <c r="O9" t="n">
         <v>0.8194444444444444</v>
       </c>
-      <c r="E9" t="n">
+      <c r="P9" t="n">
+        <v>0.7638888888888888</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="T9" t="n">
         <v>0.7222222222222222</v>
       </c>
-      <c r="F9" t="n">
-        <v>0.5416666666666666</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.5694444444444444</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.7222222222222222</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.4444444444444444</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.4444444444444444</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0.6805555555555556</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0.7222222222222222</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0.6944444444444444</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0.7777777777777778</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>0.7361111111111112</v>
-      </c>
-      <c r="R9" t="n">
-        <v>0.6944444444444444</v>
-      </c>
-      <c r="S9" t="n">
-        <v>0.7361111111111112</v>
-      </c>
-      <c r="T9" t="n">
-        <v>0.8194444444444444</v>
-      </c>
       <c r="U9" t="n">
-        <v>0.8194444444444444</v>
+        <v>0.7638888888888888</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -1026,61 +1026,61 @@
         <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4444444444444444</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E10" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.7638888888888888</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.7222222222222222</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.5277777777777778</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.5277777777777778</v>
+      </c>
+      <c r="K10" t="n">
         <v>0.6527777777777778</v>
       </c>
-      <c r="F10" t="n">
-        <v>0.5833333333333334</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.5416666666666666</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.4722222222222222</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.4722222222222222</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.5138888888888888</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0.6666666666666666</v>
-      </c>
       <c r="L10" t="n">
-        <v>0.7777777777777778</v>
+        <v>0.5972222222222222</v>
       </c>
       <c r="M10" t="n">
-        <v>0.625</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="N10" t="n">
-        <v>0.6527777777777778</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="O10" t="n">
-        <v>0.7638888888888888</v>
+        <v>0.7916666666666666</v>
       </c>
       <c r="P10" t="n">
-        <v>0.7777777777777778</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.6944444444444444</v>
       </c>
       <c r="R10" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.75</v>
       </c>
       <c r="S10" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.7361111111111112</v>
       </c>
       <c r="T10" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.7361111111111112</v>
       </c>
       <c r="U10" t="n">
-        <v>0.8472222222222222</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1092,58 +1092,58 @@
         <v>0.4444444444444444</v>
       </c>
       <c r="D11" t="n">
-        <v>0.7083333333333334</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5277777777777778</v>
+        <v>0.5</v>
       </c>
       <c r="F11" t="n">
-        <v>0.6111111111111112</v>
+        <v>0.6944444444444444</v>
       </c>
       <c r="G11" t="n">
         <v>0.8055555555555556</v>
       </c>
       <c r="H11" t="n">
-        <v>0.7638888888888888</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="I11" t="n">
-        <v>0.5694444444444444</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="J11" t="n">
-        <v>0.8055555555555556</v>
+        <v>0.8194444444444444</v>
       </c>
       <c r="K11" t="n">
-        <v>0.8055555555555556</v>
+        <v>0.6805555555555556</v>
       </c>
       <c r="L11" t="n">
-        <v>0.7638888888888888</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="M11" t="n">
-        <v>0.7638888888888888</v>
+        <v>0.6944444444444444</v>
       </c>
       <c r="N11" t="n">
-        <v>0.8055555555555556</v>
+        <v>0.6944444444444444</v>
       </c>
       <c r="O11" t="n">
-        <v>0.8055555555555556</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="P11" t="n">
-        <v>0.7638888888888888</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.7777777777777778</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="R11" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.6805555555555556</v>
       </c>
       <c r="S11" t="n">
-        <v>0.7361111111111112</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="T11" t="n">
-        <v>0.7083333333333334</v>
+        <v>0.6944444444444444</v>
       </c>
       <c r="U11" t="n">
-        <v>0.7916666666666666</v>
+        <v>0.7222222222222222</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1152,61 +1152,61 @@
         <v>4</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4444444444444444</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="D12" t="n">
-        <v>0.4444444444444444</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E12" t="n">
-        <v>0.4444444444444444</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="F12" t="n">
-        <v>0.6944444444444444</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="G12" t="n">
+        <v>0.4027777777777778</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.6527777777777778</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.7361111111111112</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.6527777777777778</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.6527777777777778</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.6527777777777778</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.6527777777777778</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.6527777777777778</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.6527777777777778</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.8055555555555556</v>
+      </c>
+      <c r="Q12" t="n">
         <v>0.7638888888888888</v>
       </c>
-      <c r="H12" t="n">
-        <v>0.6805555555555556</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0.7777777777777778</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.7222222222222222</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0.7777777777777778</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0.7361111111111112</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0.7222222222222222</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0.7361111111111112</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0.7777777777777778</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>0.7361111111111112</v>
-      </c>
       <c r="R12" t="n">
+        <v>0.8055555555555556</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.7916666666666666</v>
+      </c>
+      <c r="T12" t="n">
         <v>0.7638888888888888</v>
       </c>
-      <c r="S12" t="n">
-        <v>0.7222222222222222</v>
-      </c>
-      <c r="T12" t="n">
-        <v>0.7361111111111112</v>
-      </c>
       <c r="U12" t="n">
-        <v>0.7361111111111112</v>
+        <v>0.8472222222222222</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -1221,55 +1221,55 @@
         <v>0.5555555555555556</v>
       </c>
       <c r="E13" t="n">
-        <v>0.5694444444444444</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="F13" t="n">
-        <v>0.5277777777777778</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="G13" t="n">
-        <v>0.6527777777777778</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="H13" t="n">
-        <v>0.5277777777777778</v>
+        <v>0.5</v>
       </c>
       <c r="I13" t="n">
         <v>0.8055555555555556</v>
       </c>
       <c r="J13" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.7638888888888888</v>
+      </c>
+      <c r="L13" t="n">
         <v>0.8055555555555556</v>
       </c>
-      <c r="K13" t="n">
+      <c r="M13" t="n">
         <v>0.8055555555555556</v>
       </c>
-      <c r="L13" t="n">
+      <c r="N13" t="n">
         <v>0.7638888888888888</v>
       </c>
-      <c r="M13" t="n">
-        <v>0.8194444444444444</v>
-      </c>
-      <c r="N13" t="n">
+      <c r="O13" t="n">
+        <v>0.8055555555555556</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.7638888888888888</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.8055555555555556</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.8055555555555556</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.7361111111111112</v>
+      </c>
+      <c r="T13" t="n">
         <v>0.7916666666666666</v>
       </c>
-      <c r="O13" t="n">
-        <v>0.7916666666666666</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0.7777777777777778</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>0.6527777777777778</v>
-      </c>
-      <c r="R13" t="n">
-        <v>0.7361111111111112</v>
-      </c>
-      <c r="S13" t="n">
-        <v>0.8194444444444444</v>
-      </c>
-      <c r="T13" t="n">
-        <v>0.75</v>
-      </c>
       <c r="U13" t="n">
-        <v>0.7777777777777778</v>
+        <v>0.7638888888888888</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -1278,61 +1278,61 @@
         <v>22</v>
       </c>
       <c r="C14" t="n">
-        <v>0.4888888888888889</v>
+        <v>0.5333333333333334</v>
       </c>
       <c r="D14" t="n">
-        <v>0.6</v>
+        <v>0.5222222222222221</v>
       </c>
       <c r="E14" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.5333333333333334</v>
       </c>
       <c r="F14" t="n">
-        <v>0.5916666666666666</v>
+        <v>0.6305555555555555</v>
       </c>
       <c r="G14" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6611111111111111</v>
       </c>
       <c r="H14" t="n">
-        <v>0.6333333333333333</v>
+        <v>0.6361111111111111</v>
       </c>
       <c r="I14" t="n">
-        <v>0.675</v>
+        <v>0.6833333333333333</v>
       </c>
       <c r="J14" t="n">
-        <v>0.6583333333333334</v>
+        <v>0.6333333333333334</v>
       </c>
       <c r="K14" t="n">
-        <v>0.7</v>
+        <v>0.7027777777777777</v>
       </c>
       <c r="L14" t="n">
-        <v>0.7444444444444445</v>
+        <v>0.6861111111111111</v>
       </c>
       <c r="M14" t="n">
-        <v>0.7305555555555555</v>
+        <v>0.7277777777777776</v>
       </c>
       <c r="N14" t="n">
-        <v>0.736111111111111</v>
+        <v>0.7249999999999999</v>
       </c>
       <c r="O14" t="n">
-        <v>0.7555555555555554</v>
+        <v>0.7583333333333334</v>
       </c>
       <c r="P14" t="n">
-        <v>0.775</v>
+        <v>0.7527777777777778</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.725</v>
+        <v>0.7472222222222221</v>
       </c>
       <c r="R14" t="n">
-        <v>0.75</v>
+        <v>0.7583333333333332</v>
       </c>
       <c r="S14" t="n">
         <v>0.736111111111111</v>
       </c>
       <c r="T14" t="n">
-        <v>0.7361111111111112</v>
+        <v>0.7416666666666666</v>
       </c>
       <c r="U14" t="n">
-        <v>0.7944444444444444</v>
+        <v>0.7694444444444445</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1341,61 +1341,61 @@
         <v>23</v>
       </c>
       <c r="C15" t="n">
-        <v>0.05443310539518176</v>
+        <v>0.04444444444444447</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1431027430265695</v>
+        <v>0.04444444444444447</v>
       </c>
       <c r="E15" t="n">
-        <v>0.09662515072736715</v>
+        <v>0.02721655269759088</v>
       </c>
       <c r="F15" t="n">
-        <v>0.05931710140017395</v>
+        <v>0.08407081083567527</v>
       </c>
       <c r="G15" t="n">
-        <v>0.1039349274103873</v>
+        <v>0.1567907310185565</v>
       </c>
       <c r="H15" t="n">
-        <v>0.1133796201775475</v>
+        <v>0.1014554575986093</v>
       </c>
       <c r="I15" t="n">
-        <v>0.1307622477326647</v>
+        <v>0.1240395197875895</v>
       </c>
       <c r="J15" t="n">
-        <v>0.151025302434091</v>
+        <v>0.1026651034032018</v>
       </c>
       <c r="K15" t="n">
-        <v>0.1376612410373763</v>
+        <v>0.05091750772173153</v>
       </c>
       <c r="L15" t="n">
-        <v>0.03469443332443552</v>
+        <v>0.07168604389202189</v>
       </c>
       <c r="M15" t="n">
-        <v>0.06370747189544285</v>
+        <v>0.05597067133224969</v>
       </c>
       <c r="N15" t="n">
-        <v>0.05760122598146589</v>
+        <v>0.04922234762963707</v>
       </c>
       <c r="O15" t="n">
-        <v>0.04859126579037751</v>
+        <v>0.06248456599556663</v>
       </c>
       <c r="P15" t="n">
-        <v>0.005555555555555581</v>
+        <v>0.03447131568330793</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.04063538566202166</v>
+        <v>0.03767961101736261</v>
       </c>
       <c r="R15" t="n">
-        <v>0.04730385101646224</v>
+        <v>0.04614791034954486</v>
       </c>
       <c r="S15" t="n">
-        <v>0.04890782461571947</v>
+        <v>0.04025382429497067</v>
       </c>
       <c r="T15" t="n">
-        <v>0.05046083923495819</v>
+        <v>0.03356401659331824</v>
       </c>
       <c r="U15" t="n">
-        <v>0.03767961101736258</v>
+        <v>0.04175915660659141</v>
       </c>
     </row>
   </sheetData>
@@ -1494,61 +1494,61 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3103448275862069</v>
+        <v>0.6896551724137931</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3103448275862069</v>
+        <v>0.4827586206896552</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3103448275862069</v>
+        <v>0.6551724137931034</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7586206896551724</v>
+        <v>0.7931034482758621</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7586206896551724</v>
+        <v>0.8620689655172413</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6896551724137931</v>
+        <v>0.6551724137931034</v>
       </c>
       <c r="I2" t="n">
-        <v>0.6551724137931034</v>
+        <v>0.8620689655172413</v>
       </c>
       <c r="J2" t="n">
-        <v>0.7586206896551724</v>
+        <v>0.6206896551724138</v>
       </c>
       <c r="K2" t="n">
-        <v>0.7241379310344828</v>
+        <v>0.8275862068965517</v>
       </c>
       <c r="L2" t="n">
-        <v>0.7586206896551724</v>
+        <v>0.8275862068965517</v>
       </c>
       <c r="M2" t="n">
-        <v>0.7931034482758621</v>
+        <v>0.8275862068965517</v>
       </c>
       <c r="N2" t="n">
-        <v>0.7931034482758621</v>
+        <v>0.896551724137931</v>
       </c>
       <c r="O2" t="n">
         <v>0.896551724137931</v>
       </c>
       <c r="P2" t="n">
-        <v>0.8620689655172413</v>
+        <v>0.9655172413793104</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.8620689655172413</v>
+        <v>0.896551724137931</v>
       </c>
       <c r="R2" t="n">
-        <v>0.896551724137931</v>
+        <v>0.9310344827586207</v>
       </c>
       <c r="S2" t="n">
-        <v>0.896551724137931</v>
+        <v>0.9310344827586207</v>
       </c>
       <c r="T2" t="n">
         <v>0.896551724137931</v>
       </c>
       <c r="U2" t="n">
-        <v>0.8620689655172413</v>
+        <v>0.9310344827586207</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -1563,55 +1563,55 @@
         <v>0.6896551724137931</v>
       </c>
       <c r="E3" t="n">
+        <v>0.6896551724137931</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.6896551724137931</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.6896551724137931</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.6896551724137931</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.5862068965517241</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.7241379310344828</v>
+      </c>
+      <c r="K3" t="n">
         <v>0.6551724137931034</v>
       </c>
-      <c r="F3" t="n">
-        <v>0.7586206896551724</v>
-      </c>
-      <c r="G3" t="n">
+      <c r="L3" t="n">
+        <v>0.6896551724137931</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.6896551724137931</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.7931034482758621</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.896551724137931</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.896551724137931</v>
+      </c>
+      <c r="Q3" t="n">
         <v>0.8620689655172413</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.6551724137931034</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.7586206896551724</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.8620689655172413</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.6206896551724138</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.6206896551724138</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.896551724137931</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.7586206896551724</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0.8275862068965517</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0.8620689655172413</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0.7931034482758621</v>
       </c>
       <c r="R3" t="n">
         <v>0.896551724137931</v>
       </c>
       <c r="S3" t="n">
-        <v>0.896551724137931</v>
+        <v>0.8620689655172413</v>
       </c>
       <c r="T3" t="n">
-        <v>0.8620689655172413</v>
+        <v>0.9310344827586207</v>
       </c>
       <c r="U3" t="n">
-        <v>0.896551724137931</v>
+        <v>0.9310344827586207</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -1620,61 +1620,61 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6896551724137931</v>
+        <v>0.3103448275862069</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6896551724137931</v>
+        <v>0.5862068965517241</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7241379310344828</v>
+        <v>0.7586206896551724</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5172413793103449</v>
+        <v>0.6206896551724138</v>
       </c>
       <c r="G4" t="n">
-        <v>0.7241379310344828</v>
+        <v>0.5862068965517241</v>
       </c>
       <c r="H4" t="n">
-        <v>0.7241379310344828</v>
+        <v>0.6551724137931034</v>
       </c>
       <c r="I4" t="n">
-        <v>0.6206896551724138</v>
+        <v>0.6551724137931034</v>
       </c>
       <c r="J4" t="n">
-        <v>0.6206896551724138</v>
+        <v>0.6551724137931034</v>
       </c>
       <c r="K4" t="n">
-        <v>0.9310344827586207</v>
+        <v>0.7586206896551724</v>
       </c>
       <c r="L4" t="n">
         <v>0.7586206896551724</v>
       </c>
       <c r="M4" t="n">
-        <v>0.6551724137931034</v>
+        <v>0.9310344827586207</v>
       </c>
       <c r="N4" t="n">
         <v>0.9310344827586207</v>
       </c>
       <c r="O4" t="n">
-        <v>0.6206896551724138</v>
+        <v>0.896551724137931</v>
       </c>
       <c r="P4" t="n">
-        <v>0.7241379310344828</v>
+        <v>0.896551724137931</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.7586206896551724</v>
+        <v>0.9310344827586207</v>
       </c>
       <c r="R4" t="n">
-        <v>0.7586206896551724</v>
+        <v>0.896551724137931</v>
       </c>
       <c r="S4" t="n">
-        <v>0.9655172413793104</v>
+        <v>0.8620689655172413</v>
       </c>
       <c r="T4" t="n">
-        <v>0.9655172413793104</v>
+        <v>0.9310344827586207</v>
       </c>
       <c r="U4" t="n">
-        <v>0.896551724137931</v>
+        <v>0.9310344827586207</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -1683,61 +1683,61 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6896551724137931</v>
+        <v>0.3103448275862069</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6896551724137931</v>
+        <v>0.4137931034482759</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5862068965517241</v>
+        <v>0.4137931034482759</v>
       </c>
       <c r="F5" t="n">
-        <v>0.5862068965517241</v>
+        <v>0.6206896551724138</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6551724137931034</v>
+        <v>0.5172413793103449</v>
       </c>
       <c r="H5" t="n">
-        <v>0.6551724137931034</v>
+        <v>0.6206896551724138</v>
       </c>
       <c r="I5" t="n">
-        <v>0.6551724137931034</v>
+        <v>0.6206896551724138</v>
       </c>
       <c r="J5" t="n">
-        <v>0.8620689655172413</v>
+        <v>0.7241379310344828</v>
       </c>
       <c r="K5" t="n">
         <v>0.6551724137931034</v>
       </c>
       <c r="L5" t="n">
-        <v>0.6551724137931034</v>
+        <v>0.7586206896551724</v>
       </c>
       <c r="M5" t="n">
         <v>0.7586206896551724</v>
       </c>
       <c r="N5" t="n">
-        <v>0.8275862068965517</v>
+        <v>0.7241379310344828</v>
       </c>
       <c r="O5" t="n">
-        <v>0.8275862068965517</v>
+        <v>0.7241379310344828</v>
       </c>
       <c r="P5" t="n">
+        <v>0.7241379310344828</v>
+      </c>
+      <c r="Q5" t="n">
         <v>0.7931034482758621</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0.8275862068965517</v>
       </c>
       <c r="R5" t="n">
         <v>0.8275862068965517</v>
       </c>
       <c r="S5" t="n">
-        <v>0.8275862068965517</v>
+        <v>0.9310344827586207</v>
       </c>
       <c r="T5" t="n">
-        <v>0.8275862068965517</v>
+        <v>0.9310344827586207</v>
       </c>
       <c r="U5" t="n">
-        <v>0.896551724137931</v>
+        <v>0.9655172413793104</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -1758,49 +1758,49 @@
         <v>0.6896551724137931</v>
       </c>
       <c r="G6" t="n">
-        <v>0.7241379310344828</v>
+        <v>0.6896551724137931</v>
       </c>
       <c r="H6" t="n">
-        <v>0.7241379310344828</v>
+        <v>0.6896551724137931</v>
       </c>
       <c r="I6" t="n">
-        <v>0.7931034482758621</v>
+        <v>0.6896551724137931</v>
       </c>
       <c r="J6" t="n">
-        <v>0.7241379310344828</v>
+        <v>0.6551724137931034</v>
       </c>
       <c r="K6" t="n">
-        <v>0.7241379310344828</v>
+        <v>0.8620689655172413</v>
       </c>
       <c r="L6" t="n">
-        <v>0.7241379310344828</v>
+        <v>0.8275862068965517</v>
       </c>
       <c r="M6" t="n">
-        <v>0.7241379310344828</v>
+        <v>0.8620689655172413</v>
       </c>
       <c r="N6" t="n">
-        <v>0.7241379310344828</v>
+        <v>0.896551724137931</v>
       </c>
       <c r="O6" t="n">
-        <v>0.7241379310344828</v>
+        <v>0.8275862068965517</v>
       </c>
       <c r="P6" t="n">
-        <v>0.7931034482758621</v>
+        <v>0.896551724137931</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.7931034482758621</v>
+        <v>0.8275862068965517</v>
       </c>
       <c r="R6" t="n">
-        <v>0.7931034482758621</v>
+        <v>0.8275862068965517</v>
       </c>
       <c r="S6" t="n">
-        <v>0.8275862068965517</v>
+        <v>0.896551724137931</v>
       </c>
       <c r="T6" t="n">
-        <v>0.8620689655172413</v>
+        <v>0.896551724137931</v>
       </c>
       <c r="U6" t="n">
-        <v>0.8620689655172413</v>
+        <v>0.896551724137931</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -1809,61 +1809,61 @@
         <v>22</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6137931034482759</v>
+        <v>0.5379310344827586</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6137931034482759</v>
+        <v>0.5724137931034483</v>
       </c>
       <c r="E7" t="n">
-        <v>0.5931034482758621</v>
+        <v>0.6413793103448275</v>
       </c>
       <c r="F7" t="n">
+        <v>0.6827586206896552</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.6689655172413793</v>
+      </c>
+      <c r="H7" t="n">
         <v>0.6620689655172414</v>
       </c>
-      <c r="G7" t="n">
-        <v>0.7448275862068965</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.6896551724137931</v>
-      </c>
       <c r="I7" t="n">
-        <v>0.696551724137931</v>
+        <v>0.6827586206896551</v>
       </c>
       <c r="J7" t="n">
-        <v>0.7655172413793102</v>
+        <v>0.6758620689655173</v>
       </c>
       <c r="K7" t="n">
-        <v>0.7310344827586207</v>
+        <v>0.7517241379310343</v>
       </c>
       <c r="L7" t="n">
-        <v>0.7034482758620689</v>
+        <v>0.7724137931034483</v>
       </c>
       <c r="M7" t="n">
-        <v>0.7655172413793104</v>
+        <v>0.8137931034482758</v>
       </c>
       <c r="N7" t="n">
-        <v>0.8068965517241379</v>
+        <v>0.8482758620689654</v>
       </c>
       <c r="O7" t="n">
-        <v>0.7793103448275861</v>
+        <v>0.8482758620689654</v>
       </c>
       <c r="P7" t="n">
-        <v>0.8068965517241379</v>
+        <v>0.8758620689655172</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.8068965517241379</v>
+        <v>0.8620689655172414</v>
       </c>
       <c r="R7" t="n">
-        <v>0.8344827586206897</v>
+        <v>0.8758620689655172</v>
       </c>
       <c r="S7" t="n">
-        <v>0.8827586206896552</v>
+        <v>0.8965517241379309</v>
       </c>
       <c r="T7" t="n">
-        <v>0.8827586206896552</v>
+        <v>0.9172413793103449</v>
       </c>
       <c r="U7" t="n">
-        <v>0.8827586206896552</v>
+        <v>0.9310344827586207</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -1872,61 +1872,61 @@
         <v>23</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1517241379310345</v>
+        <v>0.1858233597973445</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1517241379310345</v>
+        <v>0.1103448275862069</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1485562705416415</v>
+        <v>0.1186527623040362</v>
       </c>
       <c r="F8" t="n">
+        <v>0.06320794062008056</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.1166312725881914</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.02580453370188927</v>
+      </c>
+      <c r="I8" t="n">
         <v>0.09605785018747667</v>
       </c>
-      <c r="G8" t="n">
-        <v>0.06757213083539801</v>
-      </c>
-      <c r="H8" t="n">
+      <c r="J8" t="n">
+        <v>0.04137931034482759</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.08558395617924729</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.05160906740377849</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.08333135154203151</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.07741360110566774</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.06757213083539802</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.0804269226875214</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.04876598490941706</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.04137931034482759</v>
+      </c>
+      <c r="S8" t="n">
         <v>0.03084231693103159</v>
       </c>
-      <c r="I8" t="n">
-        <v>0.06686454975746661</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.09097176522946838</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.1077275817366435</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.05602785106645489</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.07983335795027743</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.07100434579991034</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0.09655172413793102</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0.05160906740377848</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0.03516565181788126</v>
-      </c>
-      <c r="R8" t="n">
-        <v>0.05517241379310346</v>
-      </c>
-      <c r="S8" t="n">
-        <v>0.05160906740377853</v>
-      </c>
       <c r="T8" t="n">
-        <v>0.04677468953879498</v>
+        <v>0.01689303270884948</v>
       </c>
       <c r="U8" t="n">
-        <v>0.01689303270884954</v>
+        <v>0.02180881144943711</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -1949,49 +1949,49 @@
         <v>0.4838709677419355</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4838709677419355</v>
+        <v>0.7419354838709677</v>
       </c>
       <c r="H9" t="n">
         <v>0.7741935483870968</v>
       </c>
       <c r="I9" t="n">
-        <v>0.6451612903225806</v>
+        <v>0.7741935483870968</v>
       </c>
       <c r="J9" t="n">
+        <v>0.8387096774193549</v>
+      </c>
+      <c r="K9" t="n">
         <v>0.7741935483870968</v>
       </c>
-      <c r="K9" t="n">
-        <v>0.6451612903225806</v>
-      </c>
       <c r="L9" t="n">
+        <v>0.8709677419354839</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.8709677419354839</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.8709677419354839</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.7741935483870968</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.8709677419354839</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.8709677419354839</v>
+      </c>
+      <c r="R9" t="n">
         <v>0.8064516129032258</v>
       </c>
-      <c r="M9" t="n">
-        <v>0.8064516129032258</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0.8387096774193549</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0.8709677419354839</v>
-      </c>
-      <c r="P9" t="n">
+      <c r="S9" t="n">
         <v>0.9032258064516129</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="T9" t="n">
         <v>0.9032258064516129</v>
       </c>
-      <c r="R9" t="n">
+      <c r="U9" t="n">
         <v>0.9032258064516129</v>
-      </c>
-      <c r="S9" t="n">
-        <v>0.8709677419354839</v>
-      </c>
-      <c r="T9" t="n">
-        <v>0.8709677419354839</v>
-      </c>
-      <c r="U9" t="n">
-        <v>0.8064516129032258</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -2003,58 +2003,58 @@
         <v>0.4516129032258064</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4516129032258064</v>
+        <v>0.6129032258064516</v>
       </c>
       <c r="E10" t="n">
-        <v>0.4516129032258064</v>
+        <v>0.6774193548387096</v>
       </c>
       <c r="F10" t="n">
-        <v>0.4838709677419355</v>
+        <v>0.6129032258064516</v>
       </c>
       <c r="G10" t="n">
-        <v>0.6129032258064516</v>
+        <v>0.5483870967741935</v>
       </c>
       <c r="H10" t="n">
-        <v>0.6129032258064516</v>
+        <v>0.4193548387096774</v>
       </c>
       <c r="I10" t="n">
-        <v>0.8064516129032258</v>
+        <v>0.4193548387096774</v>
       </c>
       <c r="J10" t="n">
-        <v>0.8064516129032258</v>
+        <v>0.7419354838709677</v>
       </c>
       <c r="K10" t="n">
-        <v>0.7096774193548387</v>
+        <v>0.6774193548387096</v>
       </c>
       <c r="L10" t="n">
         <v>0.6774193548387096</v>
       </c>
       <c r="M10" t="n">
-        <v>0.8064516129032258</v>
+        <v>0.7419354838709677</v>
       </c>
       <c r="N10" t="n">
         <v>0.8064516129032258</v>
       </c>
       <c r="O10" t="n">
+        <v>0.8387096774193549</v>
+      </c>
+      <c r="P10" t="n">
         <v>0.8064516129032258</v>
       </c>
-      <c r="P10" t="n">
-        <v>0.6774193548387096</v>
-      </c>
       <c r="Q10" t="n">
-        <v>0.8387096774193549</v>
+        <v>0.7741935483870968</v>
       </c>
       <c r="R10" t="n">
         <v>0.8064516129032258</v>
       </c>
       <c r="S10" t="n">
-        <v>0.8064516129032258</v>
+        <v>0.7741935483870968</v>
       </c>
       <c r="T10" t="n">
-        <v>0.8064516129032258</v>
+        <v>0.8387096774193549</v>
       </c>
       <c r="U10" t="n">
-        <v>0.8387096774193549</v>
+        <v>0.8709677419354839</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -2063,61 +2063,61 @@
         <v>3</v>
       </c>
       <c r="C11" t="n">
-        <v>0.4516129032258064</v>
+        <v>0.5483870967741935</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4193548387096774</v>
+        <v>0.6451612903225806</v>
       </c>
       <c r="E11" t="n">
-        <v>0.6129032258064516</v>
+        <v>0.5161290322580645</v>
       </c>
       <c r="F11" t="n">
+        <v>0.5161290322580645</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.5161290322580645</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.5161290322580645</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.7419354838709677</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.7419354838709677</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.6451612903225806</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.7419354838709677</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.6451612903225806</v>
+      </c>
+      <c r="N11" t="n">
         <v>0.7741935483870968</v>
       </c>
-      <c r="G11" t="n">
-        <v>0.8387096774193549</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.4516129032258064</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.8387096774193549</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.8387096774193549</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0.8387096774193549</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0.8387096774193549</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0.8387096774193549</v>
-      </c>
-      <c r="N11" t="n">
-        <v>0.9032258064516129</v>
-      </c>
       <c r="O11" t="n">
-        <v>0.8709677419354839</v>
+        <v>0.8064516129032258</v>
       </c>
       <c r="P11" t="n">
-        <v>0.9032258064516129</v>
+        <v>0.8064516129032258</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.8709677419354839</v>
+        <v>0.8064516129032258</v>
       </c>
       <c r="R11" t="n">
-        <v>0.8387096774193549</v>
+        <v>0.8064516129032258</v>
       </c>
       <c r="S11" t="n">
-        <v>0.9032258064516129</v>
+        <v>0.8064516129032258</v>
       </c>
       <c r="T11" t="n">
-        <v>0.8709677419354839</v>
+        <v>0.8064516129032258</v>
       </c>
       <c r="U11" t="n">
-        <v>0.8709677419354839</v>
+        <v>0.8064516129032258</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -2126,61 +2126,61 @@
         <v>4</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4516129032258064</v>
+        <v>0.5483870967741935</v>
       </c>
       <c r="D12" t="n">
-        <v>0.2258064516129032</v>
+        <v>0.5483870967741935</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5806451612903226</v>
+        <v>0.5483870967741935</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5806451612903226</v>
+        <v>0.6129032258064516</v>
       </c>
       <c r="G12" t="n">
-        <v>0.5806451612903226</v>
+        <v>0.6451612903225806</v>
       </c>
       <c r="H12" t="n">
+        <v>0.6451612903225806</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.6451612903225806</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.6451612903225806</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.6451612903225806</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.6451612903225806</v>
+      </c>
+      <c r="M12" t="n">
         <v>0.7741935483870968</v>
       </c>
-      <c r="I12" t="n">
+      <c r="N12" t="n">
         <v>0.8064516129032258</v>
       </c>
-      <c r="J12" t="n">
-        <v>0.6774193548387096</v>
-      </c>
-      <c r="K12" t="n">
+      <c r="O12" t="n">
         <v>0.8064516129032258</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0.8387096774193549</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0.8387096774193549</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0.8387096774193549</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0.7741935483870968</v>
       </c>
       <c r="P12" t="n">
         <v>0.8064516129032258</v>
       </c>
       <c r="Q12" t="n">
+        <v>0.7741935483870968</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.7741935483870968</v>
+      </c>
+      <c r="S12" t="n">
         <v>0.8064516129032258</v>
       </c>
-      <c r="R12" t="n">
-        <v>0.967741935483871</v>
-      </c>
-      <c r="S12" t="n">
-        <v>0.9354838709677419</v>
-      </c>
       <c r="T12" t="n">
-        <v>0.9354838709677419</v>
+        <v>0.8387096774193549</v>
       </c>
       <c r="U12" t="n">
-        <v>0.9354838709677419</v>
+        <v>0.8387096774193549</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -2189,58 +2189,58 @@
         <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>0.4516129032258064</v>
+        <v>0.5483870967741935</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8387096774193549</v>
+        <v>0.5483870967741935</v>
       </c>
       <c r="E13" t="n">
-        <v>0.4838709677419355</v>
+        <v>0.5483870967741935</v>
       </c>
       <c r="F13" t="n">
-        <v>0.6451612903225806</v>
+        <v>0.5483870967741935</v>
       </c>
       <c r="G13" t="n">
-        <v>0.6774193548387096</v>
+        <v>0.5483870967741935</v>
       </c>
       <c r="H13" t="n">
-        <v>0.8387096774193549</v>
+        <v>0.5483870967741935</v>
       </c>
       <c r="I13" t="n">
-        <v>0.6451612903225806</v>
+        <v>0.5483870967741935</v>
       </c>
       <c r="J13" t="n">
         <v>0.6451612903225806</v>
       </c>
       <c r="K13" t="n">
-        <v>0.7096774193548387</v>
+        <v>0.5161290322580645</v>
       </c>
       <c r="L13" t="n">
-        <v>0.7096774193548387</v>
+        <v>0.5161290322580645</v>
       </c>
       <c r="M13" t="n">
         <v>0.7096774193548387</v>
       </c>
       <c r="N13" t="n">
+        <v>0.6451612903225806</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.6451612903225806</v>
+      </c>
+      <c r="P13" t="n">
         <v>0.8064516129032258</v>
-      </c>
-      <c r="O13" t="n">
-        <v>0.8709677419354839</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0.9032258064516129</v>
       </c>
       <c r="Q13" t="n">
         <v>0.8064516129032258</v>
       </c>
       <c r="R13" t="n">
+        <v>0.8064516129032258</v>
+      </c>
+      <c r="S13" t="n">
         <v>0.8387096774193549</v>
       </c>
-      <c r="S13" t="n">
-        <v>0.9032258064516129</v>
-      </c>
       <c r="T13" t="n">
-        <v>0.8709677419354839</v>
+        <v>0.8387096774193549</v>
       </c>
       <c r="U13" t="n">
         <v>0.8709677419354839</v>
@@ -2252,61 +2252,61 @@
         <v>22</v>
       </c>
       <c r="C14" t="n">
-        <v>0.4516129032258064</v>
+        <v>0.5096774193548387</v>
       </c>
       <c r="D14" t="n">
-        <v>0.4774193548387097</v>
+        <v>0.5612903225806452</v>
       </c>
       <c r="E14" t="n">
-        <v>0.5161290322580645</v>
+        <v>0.5483870967741935</v>
       </c>
       <c r="F14" t="n">
-        <v>0.5935483870967742</v>
+        <v>0.5548387096774193</v>
       </c>
       <c r="G14" t="n">
-        <v>0.6387096774193548</v>
+        <v>0.6</v>
       </c>
       <c r="H14" t="n">
-        <v>0.6903225806451614</v>
+        <v>0.5806451612903226</v>
       </c>
       <c r="I14" t="n">
-        <v>0.7483870967741935</v>
+        <v>0.6258064516129032</v>
       </c>
       <c r="J14" t="n">
-        <v>0.7483870967741935</v>
+        <v>0.7225806451612902</v>
       </c>
       <c r="K14" t="n">
-        <v>0.7419354838709677</v>
+        <v>0.6516129032258065</v>
       </c>
       <c r="L14" t="n">
+        <v>0.6903225806451612</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.7483870967741936</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.7806451612903225</v>
+      </c>
+      <c r="O14" t="n">
         <v>0.7741935483870968</v>
       </c>
-      <c r="M14" t="n">
+      <c r="P14" t="n">
+        <v>0.8193548387096774</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.8064516129032258</v>
+      </c>
+      <c r="R14" t="n">
         <v>0.8</v>
       </c>
-      <c r="N14" t="n">
-        <v>0.8387096774193548</v>
-      </c>
-      <c r="O14" t="n">
-        <v>0.8387096774193548</v>
-      </c>
-      <c r="P14" t="n">
-        <v>0.8387096774193548</v>
-      </c>
-      <c r="Q14" t="n">
+      <c r="S14" t="n">
+        <v>0.8258064516129032</v>
+      </c>
+      <c r="T14" t="n">
         <v>0.8451612903225806</v>
       </c>
-      <c r="R14" t="n">
-        <v>0.8709677419354838</v>
-      </c>
-      <c r="S14" t="n">
-        <v>0.8838709677419354</v>
-      </c>
-      <c r="T14" t="n">
-        <v>0.8709677419354838</v>
-      </c>
       <c r="U14" t="n">
-        <v>0.8645161290322581</v>
+        <v>0.8580645161290322</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -2315,61 +2315,61 @@
         <v>23</v>
       </c>
       <c r="C15" t="n">
-        <v>5.551115123125783e-17</v>
+        <v>0.04740947889257763</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1992702607932968</v>
+        <v>0.06642342026443226</v>
       </c>
       <c r="E15" t="n">
-        <v>0.06766508697871948</v>
+        <v>0.07355970484510566</v>
       </c>
       <c r="F15" t="n">
-        <v>0.1091066743566952</v>
+        <v>0.05161290322580646</v>
       </c>
       <c r="G15" t="n">
-        <v>0.1179075282741746</v>
+        <v>0.08312321759177502</v>
       </c>
       <c r="H15" t="n">
-        <v>0.1407575756727189</v>
+        <v>0.1206986253798045</v>
       </c>
       <c r="I15" t="n">
-        <v>0.08510261908563174</v>
+        <v>0.129996397932967</v>
       </c>
       <c r="J15" t="n">
-        <v>0.07468281872767889</v>
+        <v>0.07241917522788276</v>
       </c>
       <c r="K15" t="n">
-        <v>0.07067387838776336</v>
+        <v>0.08262095790235933</v>
       </c>
       <c r="L15" t="n">
-        <v>0.06766508697871947</v>
+        <v>0.1164869037759212</v>
       </c>
       <c r="M15" t="n">
-        <v>0.04740947889257763</v>
+        <v>0.07468281872767887</v>
       </c>
       <c r="N15" t="n">
+        <v>0.07468281872767887</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.06766508697871945</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.02580645161290325</v>
+      </c>
+      <c r="Q15" t="n">
         <v>0.03533693919388169</v>
       </c>
-      <c r="O15" t="n">
-        <v>0.04080358271185008</v>
-      </c>
-      <c r="P15" t="n">
-        <v>0.08892934678767886</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>0.03761904448287292</v>
-      </c>
       <c r="R15" t="n">
-        <v>0.05770498006451071</v>
+        <v>0.0129032258064516</v>
       </c>
       <c r="S15" t="n">
         <v>0.04375696763306625</v>
       </c>
       <c r="T15" t="n">
-        <v>0.04080358271185006</v>
+        <v>0.03160631926171843</v>
       </c>
       <c r="U15" t="n">
-        <v>0.04279515858523096</v>
+        <v>0.03289690008769539</v>
       </c>
     </row>
   </sheetData>

</xml_diff>